<commit_message>
added starred plants to populate script
</commit_message>
<xml_diff>
--- a/treebay_testing_data/users.xlsx
+++ b/treebay_testing_data/users.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\CS\2Web\TreeBay\treebay_django_project\treebay_testing_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\all\Uni\2_year_19-20\WED\Treebay\treebay_django_project\treebay_testing_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B7C8A0A-E3D0-44CE-BFA3-1BB5388819FB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416"/>
+    <workbookView xWindow="-22605" yWindow="1395" windowWidth="14400" windowHeight="7365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hárok1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>email</t>
   </si>
@@ -105,12 +106,24 @@
   </si>
   <si>
     <t>liza1234</t>
+  </si>
+  <si>
+    <t>Spiky boi</t>
+  </si>
+  <si>
+    <t>Aloe Vera</t>
+  </si>
+  <si>
+    <t>Aloe Vera, Mini palm</t>
+  </si>
+  <si>
+    <t>starred</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -154,8 +167,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Hypertextové prepojenie" xfId="1" builtinId="8"/>
+    <cellStyle name="Normálna" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -432,22 +445,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D10"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="20.21875" customWidth="1"/>
-    <col min="3" max="3" width="11.21875" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.1796875" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" customWidth="1"/>
+    <col min="4" max="4" width="20.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -457,8 +470,11 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -468,8 +484,11 @@
       <c r="C2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -480,7 +499,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -491,7 +510,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -502,7 +521,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -513,7 +532,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -523,8 +542,11 @@
       <c r="C7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -535,7 +557,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -545,17 +567,20 @@
       <c r="C9" t="s">
         <v>26</v>
       </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="B7" r:id="rId6"/>
-    <hyperlink ref="B8" r:id="rId7"/>
-    <hyperlink ref="B9" r:id="rId8"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Done some TODOs in category.html
</commit_message>
<xml_diff>
--- a/treebay_testing_data/users.xlsx
+++ b/treebay_testing_data/users.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>email</t>
   </si>
@@ -110,9 +110,6 @@
     <t>Aloe Vera</t>
   </si>
   <si>
-    <t>Aloe Vera, Mini palm</t>
-  </si>
-  <si>
     <t>starred</t>
   </si>
   <si>
@@ -122,7 +119,16 @@
     <t>Peace lily</t>
   </si>
   <si>
-    <t>Peace lily, Ficus</t>
+    <t>Peace lily, Mint pot, Ficus, Mini red rose pot</t>
+  </si>
+  <si>
+    <t>Aloe Vera, Mini palm, Mini pine tree</t>
+  </si>
+  <si>
+    <t>Aloe Vera, Purple kalanchoe, Spiky boi</t>
+  </si>
+  <si>
+    <t>Peace lily, Ficus, Aloe Vera, Mini palm</t>
   </si>
 </sst>
 </file>
@@ -462,7 +468,7 @@
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="20.21875" customWidth="1"/>
     <col min="3" max="3" width="11.21875" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" customWidth="1"/>
+    <col min="4" max="4" width="37.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -476,7 +482,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -490,7 +496,7 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -504,7 +510,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -529,7 +535,7 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -542,6 +548,9 @@
       <c r="C6" t="s">
         <v>13</v>
       </c>
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -554,7 +563,7 @@
         <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -568,7 +577,7 @@
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>